<commit_message>
Add luận đại vận
</commit_message>
<xml_diff>
--- a/Luangiaichung.xlsx
+++ b/Luangiaichung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4138759-099A-45D9-931B-A81359D20659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24519BC6-640E-4321-AF5A-F625A7EA1E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Can sinh Chi</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Bạn là người có năng lực khá đầy đủ vững chắc. Hãy cố gắng phát huy năng lực hơn nữa.</t>
   </si>
   <si>
-    <t>Cuộc đời của bạn nhiều điều không toại lòng. Hãy kiên định và cố gắng sẽ có quả ngọt.</t>
-  </si>
-  <si>
     <t>Bạn có Phúc đức quá lớn, tiềm tàng hơn người. Hãy làm việc tốt để tích thêm phước báu.</t>
   </si>
   <si>
@@ -55,6 +52,21 @@
   </si>
   <si>
     <t>Bạn gặp nhiều may mắn hơn thực lực bản thân. Hãy cố gắng trau dồi năng lực để càng gặp nhiều điều toại nguyện hơn.</t>
+  </si>
+  <si>
+    <t>Cuộc đời của bạn nhiều điều không toại lòng. Hãy kiên định và cố gắng sẽ có quả ngọt, cẩn thận trong cả lúc thuận lợi nhất.</t>
+  </si>
+  <si>
+    <t>Âm Dương Thuận Lý</t>
+  </si>
+  <si>
+    <t>Âm Dương Nghịch Lý</t>
+  </si>
+  <si>
+    <t>Độ số may mắn trong cuộc đời bị giảm đi. Bạn nên kiên nhẫn chắc chắn gặt quả ngọt sau nhiều bài học bắt buộc phải có.</t>
+  </si>
+  <si>
+    <t>Độ số may mắn trong cuộc đời bạn được gia tăng. Đừng để ưu ái của vận mệnh khiến bạn mất ý chí cố gắng mà hãy tận dụng cơ hội để nâng cao năng lực của bản thân.</t>
   </si>
 </sst>
 </file>
@@ -372,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,7 +400,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -396,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -404,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -421,6 +433,22 @@
       </c>
       <c r="B5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoàn thiện core  luận chung, từng đại vận, từng cung, lời khuyên
</commit_message>
<xml_diff>
--- a/Luangiaichung.xlsx
+++ b/Luangiaichung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24519BC6-640E-4321-AF5A-F625A7EA1E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C567D2-C797-48E6-A95B-603BE88BCEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Can sinh Chi</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>Độ số may mắn trong cuộc đời bạn được gia tăng. Đừng để ưu ái của vận mệnh khiến bạn mất ý chí cố gắng mà hãy tận dụng cơ hội để nâng cao năng lực của bản thân.</t>
+  </si>
+  <si>
+    <t>Ngũ hành bản Mệnh sinh Ngũ hành Thiên Mã</t>
+  </si>
+  <si>
+    <t>Bạn phải lao tâm, vất vả lo nghĩ về những thay đổi, bạn rất năng động và hay phải đi xa rất nhiều.</t>
+  </si>
+  <si>
+    <t>Ngũ hành bản Mệnh khắc Ngũ hành Thiên Mã</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn </t>
+  </si>
+  <si>
+    <t>Ngũ hành Thiên Mã sinh Ngũ hành bản Mệnh</t>
+  </si>
+  <si>
+    <t>Ngũ hành Thiên Mã khắc Ngũ hành bản Mệnh</t>
+  </si>
+  <si>
+    <t>Ngũ hành Thiên Mã đồng hành cùng Ngũ hành bản Mệnh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn đi lai, di chuyển an toàn, khi bạn tích cực và năng động tính toán lo lắng công việc thì mọi chuyện hanh thông. </t>
   </si>
 </sst>
 </file>
@@ -384,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +475,40 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
An tử vi tại mệnh hoàn thiện
</commit_message>
<xml_diff>
--- a/Luangiaichung.xlsx
+++ b/Luangiaichung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6706497-B47E-4298-A91A-62B67C247639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0120FBD-B9AE-4769-87A3-7112FFBD9352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Can sinh Chi</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t xml:space="preserve">Bạn là người có năng lực khá đầy đủ vững chắc. </t>
+  </si>
+  <si>
+    <t>Âm Long Trực</t>
+  </si>
+  <si>
+    <t>Bạn là người thông minh, biết cách ứng xử phù hợp và nên giữ đức tính nhu thuận làm kim chỉ nam cuộc đời để gặp nhiều may mắn. Thuận thiên vô chiến tự nhiên thành.</t>
+  </si>
+  <si>
+    <t>Tuế Hổ Phù</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn sinh ra gặp rất nhiều sóng gió cuộc đời nhưng đến khi vào đại vận trung niên bạn sẽ được hưởng trọn vẹn thành quả của những cố gắng, kiến thức, trải nghiệm đã đựợc tích lũy trước đó, cuộc sống gắn liền phần nhiều đến tín ngưỡng và tôn giáo. </t>
   </si>
 </sst>
 </file>
@@ -433,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +568,22 @@
         <v>17</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>